<commit_message>
MOP Test cases till 23
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/mode_of_payment_test_data.xlsx
+++ b/TestData/Web_POS/Billing/mode_of_payment_test_data.xlsx
@@ -108,136 +108,145 @@
     <t>TC_16</t>
   </si>
   <si>
-    <t>4VUQlK</t>
+    <t>KdYzhi</t>
   </si>
   <si>
     <t>TC_17</t>
   </si>
   <si>
+    <t>userone_p1</t>
+  </si>
+  <si>
+    <t>1mzWPD</t>
+  </si>
+  <si>
+    <t>TC_18</t>
+  </si>
+  <si>
     <t>3072606245nJ</t>
   </si>
   <si>
+    <t>usertwo_p3</t>
+  </si>
+  <si>
+    <t>m3DOdg</t>
+  </si>
+  <si>
+    <t>TC_19</t>
+  </si>
+  <si>
+    <t>TC_20</t>
+  </si>
+  <si>
+    <t>TC_21</t>
+  </si>
+  <si>
+    <t>TC_22</t>
+  </si>
+  <si>
+    <t>TC_23</t>
+  </si>
+  <si>
+    <t>TC_24</t>
+  </si>
+  <si>
+    <t>TC_25</t>
+  </si>
+  <si>
+    <t>307260624ut0</t>
+  </si>
+  <si>
+    <t>usertwo_p2</t>
+  </si>
+  <si>
+    <t>TC_26</t>
+  </si>
+  <si>
+    <t>TC_27</t>
+  </si>
+  <si>
+    <t>307260624PTe</t>
+  </si>
+  <si>
+    <t>userone_p4</t>
+  </si>
+  <si>
+    <t>TC_28</t>
+  </si>
+  <si>
+    <t>307260624uOm</t>
+  </si>
+  <si>
+    <t>userone_p5</t>
+  </si>
+  <si>
+    <t>TC_29</t>
+  </si>
+  <si>
+    <t>TC_30</t>
+  </si>
+  <si>
+    <t>TC_31</t>
+  </si>
+  <si>
+    <t>TC_32</t>
+  </si>
+  <si>
+    <t>TC_33</t>
+  </si>
+  <si>
+    <t>userone_p2</t>
+  </si>
+  <si>
+    <t>TC_34</t>
+  </si>
+  <si>
+    <t>TC_35</t>
+  </si>
+  <si>
+    <t>307260624SF2</t>
+  </si>
+  <si>
+    <t>userone_p6</t>
+  </si>
+  <si>
+    <t>TC_36</t>
+  </si>
+  <si>
+    <t>307260624cuS</t>
+  </si>
+  <si>
+    <t>userone_p7</t>
+  </si>
+  <si>
+    <t>TC_37</t>
+  </si>
+  <si>
+    <t>TC_38</t>
+  </si>
+  <si>
+    <t>TC_39</t>
+  </si>
+  <si>
+    <t>TC_40</t>
+  </si>
+  <si>
+    <t>TC_41</t>
+  </si>
+  <si>
+    <t>TC_42</t>
+  </si>
+  <si>
+    <t>TC_43</t>
+  </si>
+  <si>
+    <t>TC_44</t>
+  </si>
+  <si>
+    <t>TC_45</t>
+  </si>
+  <si>
     <t>userone_p3</t>
-  </si>
-  <si>
-    <t>TC_18</t>
-  </si>
-  <si>
-    <t>TC_19</t>
-  </si>
-  <si>
-    <t>TC_20</t>
-  </si>
-  <si>
-    <t>TC_21</t>
-  </si>
-  <si>
-    <t>TC_22</t>
-  </si>
-  <si>
-    <t>TC_23</t>
-  </si>
-  <si>
-    <t>TC_24</t>
-  </si>
-  <si>
-    <t>TC_25</t>
-  </si>
-  <si>
-    <t>307260624ut0</t>
-  </si>
-  <si>
-    <t>usertwo_p2</t>
-  </si>
-  <si>
-    <t>TC_26</t>
-  </si>
-  <si>
-    <t>userone_p1</t>
-  </si>
-  <si>
-    <t>TC_27</t>
-  </si>
-  <si>
-    <t>307260624PTe</t>
-  </si>
-  <si>
-    <t>userone_p4</t>
-  </si>
-  <si>
-    <t>TC_28</t>
-  </si>
-  <si>
-    <t>307260624uOm</t>
-  </si>
-  <si>
-    <t>userone_p5</t>
-  </si>
-  <si>
-    <t>TC_29</t>
-  </si>
-  <si>
-    <t>TC_30</t>
-  </si>
-  <si>
-    <t>TC_31</t>
-  </si>
-  <si>
-    <t>TC_32</t>
-  </si>
-  <si>
-    <t>TC_33</t>
-  </si>
-  <si>
-    <t>userone_p2</t>
-  </si>
-  <si>
-    <t>TC_34</t>
-  </si>
-  <si>
-    <t>TC_35</t>
-  </si>
-  <si>
-    <t>307260624SF2</t>
-  </si>
-  <si>
-    <t>userone_p6</t>
-  </si>
-  <si>
-    <t>TC_36</t>
-  </si>
-  <si>
-    <t>307260624cuS</t>
-  </si>
-  <si>
-    <t>userone_p7</t>
-  </si>
-  <si>
-    <t>TC_37</t>
-  </si>
-  <si>
-    <t>TC_38</t>
-  </si>
-  <si>
-    <t>TC_39</t>
-  </si>
-  <si>
-    <t>TC_40</t>
-  </si>
-  <si>
-    <t>TC_41</t>
-  </si>
-  <si>
-    <t>TC_42</t>
-  </si>
-  <si>
-    <t>TC_43</t>
-  </si>
-  <si>
-    <t>TC_44</t>
-  </si>
-  <si>
-    <t>TC_45</t>
   </si>
   <si>
     <t>TC_46</t>
@@ -536,7 +545,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
@@ -815,46 +824,49 @@
         <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2">
+        <v>123456</v>
+      </c>
+      <c r="G6">
+        <v>1000</v>
+      </c>
+      <c r="H6">
+        <v>600</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="3">
+        <v>45384</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" t="s">
         <v>32</v>
-      </c>
-      <c r="F6" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G6">
-        <v>1000</v>
-      </c>
-      <c r="H6">
-        <v>600</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -862,7 +874,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
@@ -871,7 +883,7 @@
         <v>123456</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="F7" s="2">
         <v>123456</v>
@@ -902,11 +914,14 @@
       </c>
       <c r="O7" s="3" t="s">
         <v>25</v>
+      </c>
+      <c r="P7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
@@ -953,7 +968,7 @@
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
@@ -1000,7 +1015,7 @@
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
@@ -1047,7 +1062,7 @@
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>17</v>
@@ -1094,7 +1109,7 @@
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>17</v>
@@ -1145,7 +1160,7 @@
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -1192,10 +1207,10 @@
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
@@ -1204,7 +1219,7 @@
         <v>123456</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F14" s="2">
         <v>123456</v>
@@ -1239,7 +1254,7 @@
     </row>
     <row r="15" ht="14.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -1251,7 +1266,7 @@
         <v>123456</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F15" s="2">
         <v>123456</v>
@@ -1286,10 +1301,10 @@
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
@@ -1298,7 +1313,7 @@
         <v>123456</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F16" s="2">
         <v>123456</v>
@@ -1333,10 +1348,10 @@
     </row>
     <row r="17" ht="14.25">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
@@ -1345,7 +1360,7 @@
         <v>123456</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F17" s="2">
         <v>123456</v>
@@ -1384,10 +1399,10 @@
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
@@ -1396,7 +1411,7 @@
         <v>123456</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F18" s="2">
         <v>123456</v>
@@ -1435,19 +1450,19 @@
     </row>
     <row r="19" ht="14.25">
       <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="F19" s="2">
         <v>123456</v>
@@ -1486,10 +1501,10 @@
     </row>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>18</v>
@@ -1498,7 +1513,7 @@
         <v>123456</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F20" s="2">
         <v>123456</v>
@@ -1537,10 +1552,10 @@
     </row>
     <row r="21" ht="14.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>18</v>
@@ -1549,7 +1564,7 @@
         <v>123456</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F21" s="2">
         <v>123456</v>
@@ -1588,10 +1603,10 @@
     </row>
     <row r="22" ht="14.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>18</v>
@@ -1600,7 +1615,7 @@
         <v>123456</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F22" s="2">
         <v>123456</v>
@@ -1636,7 +1651,7 @@
     </row>
     <row r="23" ht="14.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>17</v>
@@ -1684,10 +1699,10 @@
     </row>
     <row r="24" ht="14.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>18</v>
@@ -1696,7 +1711,7 @@
         <v>123456</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F24" s="2">
         <v>123456</v>
@@ -1734,10 +1749,10 @@
     </row>
     <row r="25" ht="14.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>18</v>
@@ -1746,7 +1761,7 @@
         <v>123456</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F25" s="2">
         <v>123456</v>
@@ -1781,10 +1796,10 @@
     </row>
     <row r="26" ht="14.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>18</v>
@@ -1793,7 +1808,7 @@
         <v>123456</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F26" s="2">
         <v>123456</v>
@@ -1832,19 +1847,19 @@
     </row>
     <row r="27" ht="14.25">
       <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="2">
+        <v>123456</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="F27" s="2">
         <v>123456</v>
@@ -1879,10 +1894,10 @@
     </row>
     <row r="28" ht="14.25">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>18</v>
@@ -1891,7 +1906,7 @@
         <v>123456</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F28" s="2">
         <v>123456</v>
@@ -1926,10 +1941,10 @@
     </row>
     <row r="29" ht="14.25">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>18</v>
@@ -1938,7 +1953,7 @@
         <v>123456</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F29" s="2">
         <v>123456</v>
@@ -1973,7 +1988,7 @@
     </row>
     <row r="30" ht="14.25">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>17</v>
@@ -2020,7 +2035,7 @@
     </row>
     <row r="31" ht="14.25">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>17</v>
@@ -2067,7 +2082,7 @@
     </row>
     <row r="32" ht="14.25">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>17</v>
@@ -2114,7 +2129,7 @@
     </row>
     <row r="33" ht="14.25">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>17</v>
@@ -2161,10 +2176,10 @@
     </row>
     <row r="34" ht="14.25">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>18</v>
@@ -2173,7 +2188,7 @@
         <v>123456</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="F34" s="2">
         <v>123456</v>
@@ -2208,10 +2223,10 @@
     </row>
     <row r="35" ht="14.25">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>18</v>
@@ -2220,7 +2235,7 @@
         <v>123456</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="F35" s="2">
         <v>123456</v>

</xml_diff>

<commit_message>
MOP Test cases from 24 to 32
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/mode_of_payment_test_data.xlsx
+++ b/TestData/Web_POS/Billing/mode_of_payment_test_data.xlsx
@@ -78,7 +78,7 @@
     <t>zwshashank.agrawal@teampureplay.com</t>
   </si>
   <si>
-    <t>usertwo_p1</t>
+    <t>userone_p1</t>
   </si>
   <si>
     <t>Index9QA</t>
@@ -114,9 +114,6 @@
     <t>TC_17</t>
   </si>
   <si>
-    <t>userone_p1</t>
-  </si>
-  <si>
     <t>1mzWPD</t>
   </si>
   <si>
@@ -126,21 +123,12 @@
     <t>3072606245nJ</t>
   </si>
   <si>
-    <t>usertwo_p3</t>
+    <t>userone_p3</t>
   </si>
   <si>
     <t>m3DOdg</t>
   </si>
   <si>
-    <t>TC_19</t>
-  </si>
-  <si>
-    <t>TC_20</t>
-  </si>
-  <si>
-    <t>TC_21</t>
-  </si>
-  <si>
     <t>TC_22</t>
   </si>
   <si>
@@ -150,36 +138,21 @@
     <t>TC_24</t>
   </si>
   <si>
+    <t>8906118410781 : 10 , 8906118412556 : 10</t>
+  </si>
+  <si>
     <t>TC_25</t>
   </si>
   <si>
-    <t>307260624ut0</t>
-  </si>
-  <si>
-    <t>usertwo_p2</t>
-  </si>
-  <si>
     <t>TC_26</t>
   </si>
   <si>
     <t>TC_27</t>
   </si>
   <si>
-    <t>307260624PTe</t>
-  </si>
-  <si>
-    <t>userone_p4</t>
-  </si>
-  <si>
     <t>TC_28</t>
   </si>
   <si>
-    <t>307260624uOm</t>
-  </si>
-  <si>
-    <t>userone_p5</t>
-  </si>
-  <si>
     <t>TC_29</t>
   </si>
   <si>
@@ -190,66 +163,6 @@
   </si>
   <si>
     <t>TC_32</t>
-  </si>
-  <si>
-    <t>TC_33</t>
-  </si>
-  <si>
-    <t>userone_p2</t>
-  </si>
-  <si>
-    <t>TC_34</t>
-  </si>
-  <si>
-    <t>TC_35</t>
-  </si>
-  <si>
-    <t>307260624SF2</t>
-  </si>
-  <si>
-    <t>userone_p6</t>
-  </si>
-  <si>
-    <t>TC_36</t>
-  </si>
-  <si>
-    <t>307260624cuS</t>
-  </si>
-  <si>
-    <t>userone_p7</t>
-  </si>
-  <si>
-    <t>TC_37</t>
-  </si>
-  <si>
-    <t>TC_38</t>
-  </si>
-  <si>
-    <t>TC_39</t>
-  </si>
-  <si>
-    <t>TC_40</t>
-  </si>
-  <si>
-    <t>TC_41</t>
-  </si>
-  <si>
-    <t>TC_42</t>
-  </si>
-  <si>
-    <t>TC_43</t>
-  </si>
-  <si>
-    <t>TC_44</t>
-  </si>
-  <si>
-    <t>TC_45</t>
-  </si>
-  <si>
-    <t>userone_p3</t>
-  </si>
-  <si>
-    <t>TC_46</t>
   </si>
 </sst>
 </file>
@@ -545,7 +458,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
@@ -769,159 +682,63 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" ht="14.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G5">
-        <v>1000</v>
-      </c>
-      <c r="H5">
-        <v>600</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G6">
-        <v>1000</v>
-      </c>
-      <c r="H6">
-        <v>600</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G7">
-        <v>1000</v>
-      </c>
-      <c r="H7">
-        <v>600</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P7" t="s">
-        <v>36</v>
-      </c>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5"/>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6"/>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7"/>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
@@ -965,10 +782,13 @@
       <c r="O8" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="P8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
@@ -1012,13 +832,16 @@
       <c r="O9" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="P9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
@@ -1027,7 +850,7 @@
         <v>123456</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F10" s="2">
         <v>123456</v>
@@ -1059,158 +882,52 @@
       <c r="O10" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="P10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G11">
-        <v>1000</v>
-      </c>
-      <c r="H11">
-        <v>600</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="I11" s="1"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G12">
-        <v>1000</v>
-      </c>
-      <c r="H12">
-        <v>600</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="5"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="I12" s="1"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G13">
-        <v>1000</v>
-      </c>
-      <c r="H13">
-        <v>600</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="I13" s="1"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
@@ -1219,7 +936,7 @@
         <v>123456</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="F14" s="2">
         <v>123456</v>
@@ -1254,7 +971,7 @@
     </row>
     <row r="15" ht="14.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -1266,7 +983,7 @@
         <v>123456</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F15" s="2">
         <v>123456</v>
@@ -1298,13 +1015,17 @@
       <c r="O15" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="5"/>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
@@ -1313,7 +1034,7 @@
         <v>123456</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="F16" s="2">
         <v>123456</v>
@@ -1328,7 +1049,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>22</v>
@@ -1348,10 +1069,10 @@
     </row>
     <row r="17" ht="14.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
@@ -1360,7 +1081,7 @@
         <v>123456</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="F17" s="2">
         <v>123456</v>
@@ -1392,17 +1113,13 @@
       <c r="O17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="5"/>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
@@ -1411,7 +1128,7 @@
         <v>123456</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="F18" s="2">
         <v>123456</v>
@@ -1443,17 +1160,13 @@
       <c r="O18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="5"/>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>18</v>
@@ -1462,7 +1175,7 @@
         <v>123456</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="F19" s="2">
         <v>123456</v>
@@ -1494,17 +1207,13 @@
       <c r="O19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="5"/>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>18</v>
@@ -1513,7 +1222,7 @@
         <v>123456</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="F20" s="2">
         <v>123456</v>
@@ -1552,10 +1261,10 @@
     </row>
     <row r="21" ht="14.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>18</v>
@@ -1564,7 +1273,7 @@
         <v>123456</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="F21" s="2">
         <v>123456</v>
@@ -1603,10 +1312,10 @@
     </row>
     <row r="22" ht="14.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>18</v>
@@ -1615,7 +1324,7 @@
         <v>123456</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="F22" s="2">
         <v>123456</v>
@@ -1647,11 +1356,14 @@
       <c r="O22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="U22" s="1"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="5"/>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>17</v>
@@ -1695,14 +1407,17 @@
       <c r="O23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="U23" s="1"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="5"/>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>18</v>
@@ -1711,7 +1426,7 @@
         <v>123456</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="F24" s="2">
         <v>123456</v>
@@ -1745,528 +1460,149 @@
       </c>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
-      <c r="T24" s="5"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="5"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G25">
-        <v>1000</v>
-      </c>
-      <c r="H25">
-        <v>600</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="I25" s="1"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="U25" s="1"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G26">
-        <v>1000</v>
-      </c>
-      <c r="H26">
-        <v>600</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="5"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="I26" s="1"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="U26" s="1"/>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G27">
-        <v>1000</v>
-      </c>
-      <c r="H27">
-        <v>600</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O27" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="I27" s="1"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="5"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G28">
-        <v>1000</v>
-      </c>
-      <c r="H28">
-        <v>600</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="I28" s="1"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G29">
-        <v>1000</v>
-      </c>
-      <c r="H29">
-        <v>600</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O29" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="I29" s="1"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="5"/>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G30">
-        <v>1000</v>
-      </c>
-      <c r="H30">
-        <v>600</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L30" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O30" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="I30" s="1"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G31">
-        <v>1000</v>
-      </c>
-      <c r="H31">
-        <v>600</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L31" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O31" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="I31" s="1"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G32">
-        <v>1000</v>
-      </c>
-      <c r="H32">
-        <v>600</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L32" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O32" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="I32" s="1"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G33">
-        <v>1000</v>
-      </c>
-      <c r="H33">
-        <v>600</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L33" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="I33" s="1"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F34" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G34">
-        <v>1000</v>
-      </c>
-      <c r="H34">
-        <v>600</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L34" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N34" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O34" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="I34" s="1"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F35" s="2">
-        <v>123456</v>
-      </c>
-      <c r="G35">
-        <v>1000</v>
-      </c>
-      <c r="H35">
-        <v>600</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L35" s="3">
-        <v>45384</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N35" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O35" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="I35" s="1"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
     </row>
     <row r="36" ht="14.25">
       <c r="B36" s="2"/>
@@ -2460,22 +1796,43 @@
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="J52"/>
-      <c r="K52"/>
-      <c r="L52"/>
-    </row>
-    <row r="53" ht="12.75">
-      <c r="J53"/>
-      <c r="K53"/>
-      <c r="L53"/>
-    </row>
-    <row r="54" ht="12.75">
-      <c r="J54"/>
-      <c r="K54"/>
-      <c r="L54"/>
-    </row>
-    <row r="55" ht="12.75">
+    <row r="52" ht="14.25">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="I52" s="1"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+    </row>
+    <row r="53" ht="14.25">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="I53" s="1"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+    </row>
+    <row r="54" ht="14.25">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="I54" s="1"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
       <c r="J55"/>
       <c r="K55"/>
       <c r="L55"/>
@@ -2495,9 +1852,21 @@
       <c r="K58"/>
       <c r="L58"/>
     </row>
-    <row r="59" ht="12.75"/>
-    <row r="60" ht="12.75"/>
-    <row r="61" ht="12.75"/>
+    <row r="59" ht="12.75">
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+    </row>
+    <row r="60" ht="12.75">
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+    </row>
+    <row r="61" ht="12.75">
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+    </row>
     <row r="62" ht="12.75"/>
     <row r="63" ht="12.75"/>
     <row r="64" ht="12.75"/>
@@ -2525,6 +1894,9 @@
     <row r="86" ht="12.75"/>
     <row r="87" ht="12.75"/>
     <row r="88" ht="12.75"/>
+    <row r="89" ht="12.75"/>
+    <row r="90" ht="12.75"/>
+    <row r="91" ht="12.75"/>
   </sheetData>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Added order options, carry bag, and add to cart test cases for order module
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/mode_of_payment_test_data.xlsx
+++ b/TestData/Web_POS/Billing/mode_of_payment_test_data.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Zwing_repo\zwing-qa-automation\TestData\Web_POS\Billing\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr fullPrecision="1" calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49" count="190">
   <si>
     <t>TC_Id</t>
   </si>
@@ -111,7 +106,7 @@
     <t>TC_16</t>
   </si>
   <si>
-    <t>KdYzhi</t>
+    <t>m2mrIM</t>
   </si>
   <si>
     <t>TC_17</t>
@@ -171,19 +166,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,17 +188,42 @@
       <sz val="10"/>
       <color rgb="FF2B579A"/>
       <name val="Arial"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="gray125">
         <fgColor indexed="64"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -214,46 +236,57 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF2B579A"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF2B579A"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1">
+  <cellStyleXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1" applyFill="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="ConditionalFormatStyle" xfId="1"/>
     <cellStyle name="HeaderStyle" xfId="2"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <dxfs xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0"/>
+  <tableStyles xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0"/>
 </styleSheet>
 </file>
 
@@ -455,46 +488,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:X91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="J1">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView topLeftCell="J1" view="normal" tabSelected="1" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.63" customHeight="true" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="19.28516" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="19.28516" customWidth="1"/>
-    <col min="5" max="5" width="18.57031" customWidth="1"/>
-    <col min="6" max="6" width="14.85547" customWidth="1"/>
-    <col min="7" max="7" width="16.71094" customWidth="1"/>
-    <col min="8" max="8" width="19.14063" customWidth="1"/>
-    <col min="9" max="9" width="19.14063" customWidth="1"/>
-    <col min="10" max="10" width="39.71094" style="1" customWidth="1"/>
-    <col min="11" max="11" width="32" style="1" customWidth="1"/>
-    <col min="12" max="12" width="32" style="1" customWidth="1"/>
-    <col min="13" max="13" width="28.71094" customWidth="1"/>
-    <col min="14" max="14" width="10.71094" customWidth="1"/>
-    <col min="15" max="15" width="10.71094" customWidth="1"/>
-    <col min="16" max="16" width="19.14063" customWidth="1"/>
-    <col min="17" max="17" width="19.14063" customWidth="1"/>
+    <col min="2" max="2" width="19.27734375" customWidth="1"/>
+    <col min="3" max="3" width="43.9296875" customWidth="1"/>
+    <col min="4" max="4" width="19.27734375" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.8203125" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="8" max="9" width="19.09765625" customWidth="1"/>
+    <col min="10" max="10" width="39.640625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="31.95703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="28.75" customWidth="1"/>
+    <col min="14" max="15" width="10.70703125" customWidth="1"/>
+    <col min="16" max="17" width="19.09765625" customWidth="1"/>
     <col min="18" max="18" width="36.25" style="1" customWidth="1"/>
-    <col min="19" max="19" width="22.5" style="1" customWidth="1"/>
-    <col min="20" max="20" width="22.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="23.92969" customWidth="1"/>
-    <col min="22" max="22" width="29.45703" style="1" customWidth="1"/>
-    <col min="23" max="23" width="29.45703" style="1" customWidth="1"/>
-    <col min="24" max="24" width="29.45703" style="1" customWidth="1"/>
-    <col min="25" max="25" width="23.20703" customWidth="1"/>
+    <col min="19" max="20" width="22.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="23.9296875" customWidth="1"/>
+    <col min="22" max="24" width="29.45703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="23.20703125" customWidth="1"/>
     <col min="26" max="26" width="15" customWidth="1"/>
-    <col min="27" max="27" width="18.92969" customWidth="1"/>
+    <col min="27" max="27" width="18.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:17" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -547,7 +574,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" ht="33.75" customHeight="1">
+    <row r="2" spans="1:15" ht="33.75" customHeight="1">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -594,7 +621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" ht="19.5" customHeight="1">
+    <row r="3" spans="1:15" ht="19.5" customHeight="1">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -641,7 +668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" ht="31.5" customHeight="1">
+    <row r="4" spans="1:15" ht="31.5" customHeight="1">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -688,7 +715,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1">
+    <row r="5" spans="2:15" ht="15" customHeight="1">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -702,7 +729,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" spans="2:15" ht="15" customHeight="1">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -716,7 +743,7 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
+    <row r="7" spans="2:15" ht="15" customHeight="1">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -730,7 +757,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" ht="14.25">
+    <row r="8" spans="1:16" ht="24">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -780,7 +807,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" ht="14.25">
+    <row r="9" spans="1:16" ht="14.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -830,7 +857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" ht="14.25">
+    <row r="10" spans="1:16" ht="14.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -880,7 +907,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" ht="14.25">
+    <row r="11" spans="2:15" ht="14.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -892,7 +919,7 @@
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
     </row>
-    <row r="12" ht="14.25">
+    <row r="12" spans="2:15" ht="14.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -904,7 +931,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" ht="14.25">
+    <row r="13" spans="2:15" ht="14.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -916,7 +943,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" ht="14.25">
+    <row r="14" spans="1:15" ht="14.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -963,7 +990,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" ht="14.25">
+    <row r="15" spans="1:21" ht="14.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1014,7 +1041,7 @@
       <c r="T15" s="4"/>
       <c r="U15" s="5"/>
     </row>
-    <row r="16" ht="14.25">
+    <row r="16" spans="1:15" ht="14.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1061,7 +1088,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" ht="14.25">
+    <row r="17" spans="1:15" ht="14.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1108,7 +1135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" ht="14.25">
+    <row r="18" spans="1:15" ht="14.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1155,7 +1182,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" ht="14.25">
+    <row r="19" spans="1:15" ht="14.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1202,7 +1229,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" ht="14.25">
+    <row r="20" spans="1:21" ht="14.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1253,7 +1280,7 @@
       <c r="T20" s="4"/>
       <c r="U20" s="5"/>
     </row>
-    <row r="21" ht="14.25">
+    <row r="21" spans="1:21" ht="14.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1304,7 +1331,7 @@
       <c r="T21" s="4"/>
       <c r="U21" s="5"/>
     </row>
-    <row r="22" ht="14.25">
+    <row r="22" spans="1:21" ht="14.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1355,7 +1382,7 @@
       <c r="T22" s="4"/>
       <c r="U22" s="5"/>
     </row>
-    <row r="23" ht="14.25">
+    <row r="23" spans="1:21" ht="14.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1406,7 +1433,7 @@
       <c r="T23" s="4"/>
       <c r="U23" s="5"/>
     </row>
-    <row r="24" ht="14.25">
+    <row r="24" spans="1:21" ht="14.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1457,7 +1484,7 @@
       <c r="T24" s="4"/>
       <c r="U24" s="5"/>
     </row>
-    <row r="25" ht="14.25">
+    <row r="25" spans="2:21" ht="14.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1470,7 +1497,7 @@
       <c r="O25" s="3"/>
       <c r="U25" s="1"/>
     </row>
-    <row r="26" ht="14.25">
+    <row r="26" spans="2:21" ht="14.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1483,7 +1510,7 @@
       <c r="O26" s="3"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="27" ht="14.25">
+    <row r="27" spans="2:20" ht="14.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1498,7 +1525,7 @@
       <c r="S27" s="4"/>
       <c r="T27" s="5"/>
     </row>
-    <row r="28" ht="14.25">
+    <row r="28" spans="2:15" ht="14.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1510,7 +1537,7 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" ht="14.25">
+    <row r="29" spans="2:21" ht="14.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1526,7 +1553,7 @@
       <c r="T29" s="4"/>
       <c r="U29" s="5"/>
     </row>
-    <row r="30" ht="14.25">
+    <row r="30" spans="2:15" ht="14.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1538,7 +1565,7 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" ht="14.25">
+    <row r="31" spans="2:15" ht="14.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1550,7 +1577,7 @@
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
     </row>
-    <row r="32" ht="14.25">
+    <row r="32" spans="2:15" ht="14.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1562,7 +1589,7 @@
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
     </row>
-    <row r="33" ht="14.25">
+    <row r="33" spans="2:15" ht="14.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1574,7 +1601,7 @@
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
     </row>
-    <row r="34" ht="14.25">
+    <row r="34" spans="2:15" ht="14.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1586,7 +1613,7 @@
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
     </row>
-    <row r="35" ht="14.25">
+    <row r="35" spans="2:15" ht="14.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1598,7 +1625,7 @@
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
     </row>
-    <row r="36" ht="14.25">
+    <row r="36" spans="2:15" ht="14.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1610,7 +1637,7 @@
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
     </row>
-    <row r="37" ht="14.25">
+    <row r="37" spans="2:15" ht="14.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1622,7 +1649,7 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
     </row>
-    <row r="38" ht="14.25">
+    <row r="38" spans="2:15" ht="14.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1634,7 +1661,7 @@
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
     </row>
-    <row r="39" ht="14.25">
+    <row r="39" spans="2:15" ht="14.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1646,7 +1673,7 @@
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
     </row>
-    <row r="40" ht="14.25">
+    <row r="40" spans="2:15" ht="14.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1658,7 +1685,7 @@
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
     </row>
-    <row r="41" ht="14.25">
+    <row r="41" spans="2:15" ht="14.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1670,7 +1697,7 @@
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
     </row>
-    <row r="42" ht="14.25">
+    <row r="42" spans="2:15" ht="14.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1682,7 +1709,7 @@
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
     </row>
-    <row r="43" ht="14.25">
+    <row r="43" spans="2:15" ht="14.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1694,7 +1721,7 @@
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
     </row>
-    <row r="44" ht="14.25">
+    <row r="44" spans="2:15" ht="14.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1706,7 +1733,7 @@
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
     </row>
-    <row r="45" ht="14.25">
+    <row r="45" spans="2:15" ht="14.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1718,7 +1745,7 @@
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
     </row>
-    <row r="46" ht="14.25">
+    <row r="46" spans="2:15" ht="14.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1730,7 +1757,7 @@
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
     </row>
-    <row r="47" ht="14.25">
+    <row r="47" spans="2:15" ht="14.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1742,7 +1769,7 @@
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
     </row>
-    <row r="48" ht="14.25">
+    <row r="48" spans="2:15" ht="14.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1754,7 +1781,7 @@
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
     </row>
-    <row r="49" ht="14.25">
+    <row r="49" spans="2:15" ht="14.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1766,7 +1793,7 @@
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
     </row>
-    <row r="50" ht="14.25">
+    <row r="50" spans="2:15" ht="14.25">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -1778,7 +1805,7 @@
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
     </row>
-    <row r="51" ht="14.25">
+    <row r="51" spans="2:15" ht="14.25">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -1790,7 +1817,7 @@
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
     </row>
-    <row r="52" ht="14.25">
+    <row r="52" spans="2:15" ht="14.25">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -1802,7 +1829,7 @@
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
     </row>
-    <row r="53" ht="14.25">
+    <row r="53" spans="2:15" ht="14.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -1814,7 +1841,7 @@
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
     </row>
-    <row r="54" ht="14.25">
+    <row r="54" spans="2:15" ht="14.25">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -1826,37 +1853,37 @@
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" spans="10:12" customHeight="1">
       <c r="J55"/>
       <c r="K55"/>
       <c r="L55"/>
     </row>
-    <row r="56" ht="12.75">
+    <row r="56" spans="10:12" ht="12.75">
       <c r="J56"/>
       <c r="K56"/>
       <c r="L56"/>
     </row>
-    <row r="57" ht="12.75">
+    <row r="57" spans="10:12" ht="12.75">
       <c r="J57"/>
       <c r="K57"/>
       <c r="L57"/>
     </row>
-    <row r="58" ht="12.75">
+    <row r="58" spans="10:12" ht="12.75">
       <c r="J58"/>
       <c r="K58"/>
       <c r="L58"/>
     </row>
-    <row r="59" ht="12.75">
+    <row r="59" spans="10:12" ht="12.75">
       <c r="J59"/>
       <c r="K59"/>
       <c r="L59"/>
     </row>
-    <row r="60" ht="12.75">
+    <row r="60" spans="10:12" ht="12.75">
       <c r="J60"/>
       <c r="K60"/>
       <c r="L60"/>
     </row>
-    <row r="61" ht="12.75">
+    <row r="61" spans="10:12" ht="12.75">
       <c r="J61"/>
       <c r="K61"/>
       <c r="L61"/>
@@ -1892,6 +1919,8 @@
     <row r="90" ht="12.75"/>
     <row r="91" ht="12.75"/>
   </sheetData>
-  <headerFooter alignWithMargins="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>
+  <extLst/>
 </worksheet>
 </file>
</xml_diff>